<commit_message>
modelo rodando com alterações (antes de retirar duplicidade)
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,6 +24,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$H$17</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
@@ -38,6 +40,8 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -935,34 +939,33 @@
   </sheetPr>
   <dimension ref="A1:R65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
-      <selection pane="bottomRight" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="40.0918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="12.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="39.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.4183673469388"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.02040816326531"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.31632653061224"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="3.78061224489796"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="9.85204081632653"/>
     <col collapsed="false" hidden="false" max="1023" min="19" style="1" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.0765306122449"/>
   </cols>
@@ -4927,17 +4930,16 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5007,14 +5009,14 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.75"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.77551020408163"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -5106,7 +5108,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5155,11 +5157,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
generalizando geração dos gráficos
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,6 +26,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$H$17</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
@@ -42,6 +44,8 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -939,33 +943,33 @@
   </sheetPr>
   <dimension ref="A1:R65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="39.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1479591836735"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.75"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.04591836734694"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.20918367346939"/>
     <col collapsed="false" hidden="false" max="14" min="13" style="1" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="1" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="9.58673469387755"/>
     <col collapsed="false" hidden="false" max="1023" min="19" style="1" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.0765306122449"/>
   </cols>
@@ -4930,16 +4934,17 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5009,14 +5014,14 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.47959183673469"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.36734693877551"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -5108,7 +5113,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5157,10 +5162,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Implementando Filtro das Variáveis
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,9 +13,10 @@
     <sheet name="levers" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="configs" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="VariableNames" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="RangesPlausiveis" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$H$17</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">params!$A$1:$O$78</definedName>
@@ -28,24 +29,30 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -57,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="216">
   <si>
     <t xml:space="preserve">Variavel</t>
   </si>
@@ -690,6 +697,21 @@
   </si>
   <si>
     <t xml:space="preserve">Replicação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fIndustryOrderRate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sPrice1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sPrice2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sPrice3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sPrice4</t>
   </si>
 </sst>
 </file>
@@ -948,28 +970,26 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C54" activeCellId="0" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="38.2040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="36.8520408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.3418367346939"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.3469387755102"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="1" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="1" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="9.17857142857143"/>
     <col collapsed="false" hidden="false" max="1023" min="19" style="1" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.0765306122449"/>
   </cols>
@@ -4934,17 +4954,16 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5013,15 +5032,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.96428571428571"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -5088,7 +5105,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G15"/>
+  <autoFilter ref="A1:H17"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -5113,7 +5130,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5162,11 +5179,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5316,4 +5332,103 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.0714285714286"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <f aca="false">12000*1.5^10</f>
+        <v>691980.46875</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <f aca="false">200000*4</f>
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <f aca="false">200000*4</f>
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <f aca="false">200000*4</f>
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <f aca="false">200000*4</f>
+        <v>800000</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Custo Médio Patente 6 mi, incerto
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
     <sheet name="RangesPlausiveis" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$G$15</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">params!$A$1:$O$78</definedName>
@@ -32,27 +32,29 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -965,31 +967,31 @@
   </sheetPr>
   <dimension ref="A1:R65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C54" activeCellId="0" sqref="C54"/>
+      <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="36.8520408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="36.4489795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.9234693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.0714285714286"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.20918367346939"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="14" min="11" style="1" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="1" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="9.04591836734694"/>
     <col collapsed="false" hidden="false" max="1023" min="19" style="1" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.0765306122449"/>
   </cols>
@@ -2925,11 +2927,11 @@
       </c>
       <c r="C37" s="2" t="n">
         <f aca="false">IF(I37="Incerto",MAX(G37,J37-(ABS(F37*J37))),J37)</f>
-        <v>100000</v>
+        <v>3000000</v>
       </c>
       <c r="D37" s="2" t="n">
         <f aca="false">IF(I37="Incerto",MIN(H37,J37+(ABS(F37*J37))),J37)</f>
-        <v>100000</v>
+        <v>9000000</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>115</v>
@@ -2939,17 +2941,17 @@
       </c>
       <c r="G37" s="1" t="n">
         <f aca="false">J37/4</f>
-        <v>25000</v>
+        <v>1500000</v>
       </c>
       <c r="H37" s="1" t="n">
         <f aca="false">J37*4</f>
-        <v>400000</v>
+        <v>24000000</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J37" s="1" t="n">
-        <v>100000</v>
+        <v>6000000</v>
       </c>
       <c r="K37" s="1" t="n">
         <v>100000</v>
@@ -2959,7 +2961,7 @@
       <c r="N37" s="0"/>
       <c r="O37" s="1" t="n">
         <f aca="false">D37&gt;C37</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P37" s="1" t="s">
         <v>39</v>
@@ -4960,10 +4962,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5033,12 +5036,12 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.83163265306122"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -5105,7 +5108,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H17"/>
+  <autoFilter ref="A1:G15"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -5129,9 +5132,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
@@ -5179,10 +5179,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5341,14 +5341,14 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
rodando análise prim com o python
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
     <sheet name="RangesPlausiveis" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$H$17</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">params!$A$1:$O$78</definedName>
@@ -33,28 +33,30 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -967,31 +969,29 @@
   </sheetPr>
   <dimension ref="A1:R65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
-      <selection pane="bottomRight" activeCell="D30" activeCellId="0" sqref="D30"/>
+      <selection pane="bottomRight" activeCell="F37" activeCellId="0" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="36.4489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.9234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.9081632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.8010204081633"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.10204081632653"/>
     <col collapsed="false" hidden="false" max="14" min="11" style="1" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="1" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="8.77551020408163"/>
     <col collapsed="false" hidden="false" max="1023" min="19" style="1" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.0765306122449"/>
   </cols>
@@ -2927,11 +2927,11 @@
       </c>
       <c r="C37" s="2" t="n">
         <f aca="false">IF(I37="Incerto",MAX(G37,J37-(ABS(F37*J37))),J37)</f>
-        <v>3000000</v>
+        <v>1500000</v>
       </c>
       <c r="D37" s="2" t="n">
         <f aca="false">IF(I37="Incerto",MIN(H37,J37+(ABS(F37*J37))),J37)</f>
-        <v>9000000</v>
+        <v>4500000</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>115</v>
@@ -2941,17 +2941,17 @@
       </c>
       <c r="G37" s="1" t="n">
         <f aca="false">J37/4</f>
-        <v>1500000</v>
+        <v>750000</v>
       </c>
       <c r="H37" s="1" t="n">
         <f aca="false">J37*4</f>
-        <v>24000000</v>
+        <v>12000000</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>38</v>
       </c>
       <c r="J37" s="1" t="n">
-        <v>6000000</v>
+        <v>3000000</v>
       </c>
       <c r="K37" s="1" t="n">
         <v>100000</v>
@@ -4954,19 +4954,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5005,10 +5005,21 @@
         <v>0.5</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.45</v>
+        <v>0.3</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -5036,12 +5047,12 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.69387755102041"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -5108,7 +5119,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G15"/>
+  <autoFilter ref="A1:H17"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -5132,6 +5143,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
@@ -5179,10 +5193,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5347,8 +5362,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Calibração Inicial: Mudanças Importantes
aInitialReorderShare: Agora é calculado em função da Base de Equipamentos Instalada Inicial;
InstalledBaseIni: Agora depende diretamente da Base de equipamentos instalada inicialmente.
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
     <sheet name="RangesPlausiveis" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$H$17</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">params!$A$1:$O$78</definedName>
@@ -35,30 +35,32 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -70,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="217">
   <si>
     <t xml:space="preserve">Variavel</t>
   </si>
@@ -718,6 +720,9 @@
   </si>
   <si>
     <t xml:space="preserve">sPrice4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VariacaoDemanda</t>
   </si>
 </sst>
 </file>
@@ -971,7 +976,7 @@
   </sheetPr>
   <dimension ref="A1:R65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -981,19 +986,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.3673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.530612244898"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="9" min="7" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="7.83163265306122"/>
     <col collapsed="false" hidden="false" max="14" min="11" style="1" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="1" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="8.36734693877551"/>
     <col collapsed="false" hidden="false" max="1023" min="19" style="1" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.0765306122449"/>
   </cols>
@@ -4964,11 +4969,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5049,12 +5054,12 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.4234693877551"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -5121,7 +5126,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G15"/>
+  <autoFilter ref="A1:H17"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -5146,7 +5151,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5195,11 +5200,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5356,16 +5361,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5437,6 +5442,17 @@
       <c r="C6" s="0" t="n">
         <f aca="false">200000*4</f>
         <v>800000</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajustando forma de inicialização do cumulative adopters
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="220">
   <si>
     <t>Variavel</t>
   </si>
@@ -731,6 +731,18 @@
   </si>
   <si>
     <t>VariacaoDemanda</t>
+  </si>
+  <si>
+    <t>aModoInitialCumulativeAdopters</t>
+  </si>
+  <si>
+    <t>Modo de Inicialização dos Cumulative Adopters</t>
+  </si>
+  <si>
+    <t>1 - Tradicional: Industry Demand X Initial Diffusion Fraction (Sterman)
+2 - ReorderShare -&gt; Intalled Base -&gt; Adopters (Novo)
+3 - ReorderShare -&gt; InitialAdoptionRate -&gt; Initial Cumulative Adopters (Implementado Inicialmente)
+}</t>
   </si>
 </sst>
 </file>
@@ -822,7 +834,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -844,6 +856,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1226,13 +1241,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMI78"/>
+  <dimension ref="A1:AMI79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="C40" sqref="C40"/>
+      <selection pane="bottomRight" activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,7 +1263,7 @@
     <col min="11" max="14" width="6.140625" style="1"/>
     <col min="15" max="15" width="3.5703125" style="1"/>
     <col min="16" max="16" width="15.140625" style="1"/>
-    <col min="17" max="17" width="18.140625" style="1"/>
+    <col min="17" max="17" width="36" style="1" customWidth="1"/>
     <col min="18" max="18" width="8" style="1"/>
     <col min="19" max="1023" width="6.140625" style="1"/>
     <col min="1024" max="1025" width="6.140625"/>
@@ -5191,6 +5206,47 @@
       </c>
       <c r="P78" s="1" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C79" s="2">
+        <v>2</v>
+      </c>
+      <c r="D79" s="2">
+        <v>2</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F79" s="2">
+        <v>0</v>
+      </c>
+      <c r="G79" s="1">
+        <v>1</v>
+      </c>
+      <c r="H79" s="2">
+        <v>3</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J79" s="2">
+        <v>2</v>
+      </c>
+      <c r="K79" s="1">
+        <v>1</v>
+      </c>
+      <c r="P79" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q79" s="19" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementando inicialização nova - antes de salvar resultados
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
@@ -1247,7 +1247,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="A79" sqref="A79"/>
+      <selection pane="bottomRight" activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5216,9 +5216,11 @@
         <v>218</v>
       </c>
       <c r="C79" s="2">
+        <f t="shared" ref="C79" si="14">IF(I79="Incerto",MAX(G79,J79-(ABS(F79*J79))),J79)</f>
         <v>2</v>
       </c>
       <c r="D79" s="2">
+        <f t="shared" ref="D79" si="15">IF(I79="Incerto",MIN(H79,J79+(ABS(F79*J79))),J79)</f>
         <v>2</v>
       </c>
       <c r="E79" s="1" t="s">

</xml_diff>

<commit_message>
encontrada inconsistencia no modulo de patentes
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
@@ -1244,22 +1244,21 @@
   <dimension ref="A1:AMI79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="G79" sqref="G79"/>
+      <selection pane="bottomRight" activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" style="1"/>
     <col min="2" max="2" width="33.7109375" style="1"/>
-    <col min="3" max="3" width="9.7109375" style="2"/>
-    <col min="4" max="4" width="10.5703125" style="2"/>
-    <col min="5" max="5" width="10.140625" style="1"/>
-    <col min="6" max="6" width="6.140625" style="2"/>
-    <col min="7" max="9" width="6.140625" style="1"/>
-    <col min="10" max="10" width="7.42578125" style="1"/>
+    <col min="3" max="4" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="2" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="14" width="6.140625" style="1"/>
     <col min="15" max="15" width="3.5703125" style="1"/>
     <col min="16" max="16" width="15.140625" style="1"/>
@@ -4885,7 +4884,7 @@
         <v>38</v>
       </c>
       <c r="J72" s="1">
-        <v>1.5</v>
+        <v>1.49</v>
       </c>
       <c r="K72" s="1">
         <v>1</v>
@@ -4933,7 +4932,7 @@
         <v>38</v>
       </c>
       <c r="J73" s="1">
-        <v>1.5</v>
+        <v>1.49</v>
       </c>
       <c r="K73" s="1">
         <v>1</v>
@@ -4981,7 +4980,7 @@
         <v>38</v>
       </c>
       <c r="J74" s="1">
-        <v>1.5</v>
+        <v>1.49</v>
       </c>
       <c r="K74" s="1">
         <v>1</v>
@@ -5263,7 +5262,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5300,7 +5299,7 @@
         <v>0.3</v>
       </c>
       <c r="D2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5314,7 +5313,7 @@
         <v>0.35</v>
       </c>
       <c r="D3">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
estoques iniciais considerando modo de inicialização dos cumulative adopters
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
@@ -12,63 +12,85 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="params" sheetId="1" r:id="rId1"/>
-    <sheet name="Levers_FullDesign" sheetId="2" r:id="rId2"/>
-    <sheet name="levers" sheetId="3" r:id="rId3"/>
-    <sheet name="configs" sheetId="4" r:id="rId4"/>
-    <sheet name="VariableNames" sheetId="5" r:id="rId5"/>
-    <sheet name="RangesPlausiveis" sheetId="6" r:id="rId6"/>
+    <sheet name="params_testeithink" sheetId="7" r:id="rId1"/>
+    <sheet name="params" sheetId="1" r:id="rId2"/>
+    <sheet name="Levers_FullDesign" sheetId="2" r:id="rId3"/>
+    <sheet name="levers" sheetId="3" r:id="rId4"/>
+    <sheet name="configs" sheetId="4" r:id="rId5"/>
+    <sheet name="VariableNames" sheetId="5" r:id="rId6"/>
+    <sheet name="RangesPlausiveis" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_FilterDatabase_0" localSheetId="2">levers!$A$1:$G$15</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="2">levers!$A$1:$H$17</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="2">levers!$A$1:$G$15</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="2">levers!$A$1:$H$17</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="2">levers!$A$1:$G$15</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$H$17</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$G$15</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$H$17</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$G$15</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$H$17</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$G$15</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$H$17</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$G$15</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$H$17</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$G$15</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$H$17</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$G$15</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$H$17</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$G$15</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$H$17</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params!$A$1:$O$78</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$G$15</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$H$17</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$G$15</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$H$17</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$G$15</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$H$17</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="2">levers!$A$1:$G$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2">levers!$A$1:$H$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="3">levers!$A$1:$G$15</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="3">levers!$A$1:$H$17</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="3">levers!$A$1:$G$15</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="3">levers!$A$1:$H$17</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="3">levers!$A$1:$G$15</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$H$17</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$G$15</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$H$17</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$G$15</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$H$17</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$G$15</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$H$17</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$G$15</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$H$17</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$G$15</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$H$17</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$G$15</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$H$17</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$G$15</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$H$17</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$G$15</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$H$17</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$G$15</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$H$17</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$G$15</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$H$17</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">levers!$A$1:$G$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3">levers!$A$1:$H$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">params!$A$1:$O$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">params_testeithink!$A$1:$O$78</definedName>
   </definedNames>
   <calcPr calcId="171027" iterateDelta="1E-4"/>
   <extLst>
@@ -80,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="223">
   <si>
     <t>Variavel</t>
   </si>
@@ -743,6 +765,15 @@
 2 - ReorderShare -&gt; Intalled Base -&gt; Adopters (Novo)
 3 - ReorderShare -&gt; InitialAdoptionRate -&gt; Initial Cumulative Adopters (Implementado Inicialmente)
 }</t>
+  </si>
+  <si>
+    <t>aInitialPatentLefts</t>
+  </si>
+  <si>
+    <t>Número Inicial de Patentes Abertas de Impressoras Profissionais.</t>
+  </si>
+  <si>
+    <t>patentes</t>
   </si>
 </sst>
 </file>
@@ -1240,14 +1271,4100 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMI79"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8BAED30-A0E2-440E-98B6-19A75F1BE944}">
+  <dimension ref="A1:AMI84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="I77" sqref="I77"/>
+      <selection pane="bottomRight" activeCell="A84" sqref="A84"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="4" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="2" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="9.140625" style="1"/>
+    <col min="17" max="17" width="36" style="1" customWidth="1"/>
+    <col min="18" max="1023" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2">
+        <f t="shared" ref="C2:C22" si="0">IF(I2="Incerto",MAX(G2,J2-(ABS(F2*J2))),J2)</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <f t="shared" ref="D2:D22" si="1">IF(I2="Incerto",MIN(H2,J2+(ABS(F2*J2))),J2)</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>30</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2" s="1" t="b">
+        <f t="shared" ref="N2:N34" si="2">C2=D2</f>
+        <v>1</v>
+      </c>
+      <c r="O2" s="1" t="b">
+        <f t="shared" ref="O2:O65" si="3">D2&gt;C2</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" si="1"/>
+        <v>0.04</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3">
+        <v>0.04</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O3" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G4">
+        <v>0.25</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4">
+        <v>0.25</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O4" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O5" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="2">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <f>1/10</f>
+        <v>0.1</v>
+      </c>
+      <c r="H6">
+        <f>1/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="5">
+        <f>1/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="L6">
+        <v>0.1</v>
+      </c>
+      <c r="M6">
+        <v>0.5</v>
+      </c>
+      <c r="N6" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>40</v>
+      </c>
+      <c r="R6"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O7" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>45</v>
+      </c>
+      <c r="R7"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>200000</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="1"/>
+        <v>200000</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G8">
+        <v>200000</v>
+      </c>
+      <c r="H8">
+        <v>200000</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="1">
+        <v>200000</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1000</v>
+      </c>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O8" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R8" s="1">
+        <f>107/0.5</f>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="2">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>25000</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <f>J10/2</f>
+        <v>25000</v>
+      </c>
+      <c r="H10">
+        <f>J10*2</f>
+        <v>100000</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="1">
+        <v>50000</v>
+      </c>
+      <c r="K10" s="1">
+        <v>60000000</v>
+      </c>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="8">
+        <f t="shared" si="1"/>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0.5</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="1"/>
+        <v>1.6</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>0.3</v>
+      </c>
+      <c r="H12">
+        <v>2.5</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>0.5</v>
+      </c>
+      <c r="M12">
+        <v>2.5</v>
+      </c>
+      <c r="N12" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="1"/>
+        <v>300000</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="2">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <f>J13/10</f>
+        <v>5000</v>
+      </c>
+      <c r="H13">
+        <f>J13*10</f>
+        <v>500000</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="5">
+        <v>50000</v>
+      </c>
+      <c r="K13" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q13"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E14"/>
+      <c r="F14" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O14" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q14"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="1"/>
+        <v>0.375</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="L15" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="N15" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q15"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O16" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q16"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H17" s="1">
+        <v>3</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M17" s="1">
+        <v>1</v>
+      </c>
+      <c r="N17" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q17"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O18" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q18"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O19" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q19"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G20" s="1">
+        <v>-20</v>
+      </c>
+      <c r="H20" s="1">
+        <v>20</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" s="1">
+        <v>-4</v>
+      </c>
+      <c r="K20" s="1">
+        <v>-4</v>
+      </c>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q20"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>-12</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="1">
+        <v>-20</v>
+      </c>
+      <c r="H21" s="1">
+        <v>20</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21" s="1">
+        <v>-8</v>
+      </c>
+      <c r="K21" s="1">
+        <v>-8</v>
+      </c>
+      <c r="L21" s="1">
+        <v>-12</v>
+      </c>
+      <c r="M21" s="1">
+        <v>-4</v>
+      </c>
+      <c r="N21" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q21"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q22"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="2">
+        <f>IF(H23="Incerto",MAX(G23,J23-(ABS(F23*J23))),J23)</f>
+        <v>20000</v>
+      </c>
+      <c r="D23" s="2">
+        <f>IF(H23="Incerto",MIN(G23,J23+(ABS(F23*J23))),J23)</f>
+        <v>20000</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="1">
+        <f>J23/2</f>
+        <v>10000</v>
+      </c>
+      <c r="H23" s="1">
+        <f>J23*2</f>
+        <v>40000</v>
+      </c>
+      <c r="I23" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="1">
+        <v>20000</v>
+      </c>
+      <c r="K23" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O23" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q23"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" ref="C24:C80" si="4">IF(I24="Incerto",MAX(G24,J24-(ABS(F24*J24))),J24)</f>
+        <v>1.5</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" ref="D24:D80" si="5">IF(I24="Incerto",MIN(H24,J24+(ABS(F24*J24))),J24)</f>
+        <v>4.5</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H24" s="1">
+        <f>J24*3</f>
+        <v>9</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J24" s="1">
+        <v>3</v>
+      </c>
+      <c r="K24" s="1">
+        <v>3</v>
+      </c>
+      <c r="L24" s="1">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M24" s="1">
+        <v>3</v>
+      </c>
+      <c r="N24" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q24"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="5"/>
+        <v>0.2</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q25"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="4"/>
+        <v>0.7</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="L26" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="M26" s="1">
+        <v>1</v>
+      </c>
+      <c r="N26" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O26" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q26"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" si="4"/>
+        <v>200</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="5"/>
+        <v>200</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="1">
+        <f>J27/2</f>
+        <v>100</v>
+      </c>
+      <c r="H27" s="1">
+        <f>J27*2</f>
+        <v>400</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27" s="1">
+        <v>200</v>
+      </c>
+      <c r="K27" s="1">
+        <v>100000</v>
+      </c>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O27" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q27"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E28"/>
+      <c r="F28" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J28" s="1">
+        <v>1</v>
+      </c>
+      <c r="K28" s="1">
+        <v>1</v>
+      </c>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O28" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q28"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O29" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q29"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H30" s="1">
+        <v>2</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J30" s="1">
+        <v>1</v>
+      </c>
+      <c r="K30" s="1">
+        <v>1</v>
+      </c>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O30" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q30"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="5"/>
+        <v>1.5</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
+        <f>J31*3</f>
+        <v>3</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J31" s="1">
+        <v>1</v>
+      </c>
+      <c r="K31" s="1">
+        <v>1</v>
+      </c>
+      <c r="L31" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M31" s="1">
+        <v>1</v>
+      </c>
+      <c r="N31" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O31" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q31"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" si="4"/>
+        <v>0.125</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="5"/>
+        <v>0.375</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <f>J32*3</f>
+        <v>0.75</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="L32" s="1">
+        <v>0</v>
+      </c>
+      <c r="M32" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="N32" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O32" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q32"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="2">
+        <f t="shared" si="4"/>
+        <v>-0.15000000000000002</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" si="5"/>
+        <v>-0.05</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G33" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J33" s="1">
+        <v>-0.1</v>
+      </c>
+      <c r="K33" s="1">
+        <v>-0.1</v>
+      </c>
+      <c r="L33" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="M33" s="1">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O33" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q33"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0</v>
+      </c>
+      <c r="K34" s="1">
+        <v>0</v>
+      </c>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O34" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q34"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="2">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1</v>
+      </c>
+      <c r="H35" s="1">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J35" s="1">
+        <v>1</v>
+      </c>
+      <c r="K35" s="1">
+        <v>0</v>
+      </c>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q35"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" s="2">
+        <f t="shared" si="4"/>
+        <v>2.5</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" si="5"/>
+        <v>7.5</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1</v>
+      </c>
+      <c r="H36" s="1">
+        <v>10</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J36" s="1">
+        <v>5</v>
+      </c>
+      <c r="K36" s="1">
+        <v>5</v>
+      </c>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q36"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" s="2">
+        <f t="shared" si="4"/>
+        <v>1500000</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" si="5"/>
+        <v>4500000</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G37" s="1">
+        <f t="shared" ref="G37:G44" si="6">J37/4</f>
+        <v>750000</v>
+      </c>
+      <c r="H37" s="1">
+        <f>J37*4</f>
+        <v>12000000</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J37" s="1">
+        <v>3000000</v>
+      </c>
+      <c r="K37" s="1">
+        <v>100000</v>
+      </c>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q37"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C38" s="2">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D38" s="2">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G38" s="1">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="H38" s="1">
+        <f>J38*4</f>
+        <v>8</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J38" s="1">
+        <v>2</v>
+      </c>
+      <c r="K38" s="1">
+        <v>2</v>
+      </c>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q38"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" s="2">
+        <f t="shared" si="4"/>
+        <v>0.2</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="5"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G39" s="1">
+        <f t="shared" si="6"/>
+        <v>0.1</v>
+      </c>
+      <c r="H39" s="1">
+        <v>1</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J39" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="K39" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="O39" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q39"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C40" s="2">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G40" s="1">
+        <f t="shared" si="6"/>
+        <v>4.5</v>
+      </c>
+      <c r="H40" s="1">
+        <f>J40*4</f>
+        <v>72</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J40" s="1">
+        <v>18</v>
+      </c>
+      <c r="K40" s="1">
+        <v>18</v>
+      </c>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="O40" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q40"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="D41" s="2">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" si="6"/>
+        <v>2.5</v>
+      </c>
+      <c r="H41" s="1">
+        <f>J41*4</f>
+        <v>40</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J41" s="1">
+        <v>10</v>
+      </c>
+      <c r="K41" s="1">
+        <v>10</v>
+      </c>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q41"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C42" s="2">
+        <f t="shared" si="4"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D42" s="2">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G42" s="1">
+        <f t="shared" si="6"/>
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="H42" s="1">
+        <f>J42*4</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J42" s="1">
+        <f>1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="K42" s="1">
+        <f>1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
+      <c r="O42" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q42"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D43" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E43"/>
+      <c r="F43" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H43" s="1">
+        <f>J43*4</f>
+        <v>0</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J43" s="1">
+        <v>0</v>
+      </c>
+      <c r="K43" s="1">
+        <v>0</v>
+      </c>
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43"/>
+      <c r="O43" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q43"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C44" s="2">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="D44" s="2">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E44"/>
+      <c r="F44" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G44" s="1">
+        <f t="shared" si="6"/>
+        <v>2.5</v>
+      </c>
+      <c r="H44" s="1">
+        <f>J44*4</f>
+        <v>40</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J44" s="1">
+        <v>10</v>
+      </c>
+      <c r="K44" s="1">
+        <v>10</v>
+      </c>
+      <c r="L44"/>
+      <c r="M44"/>
+      <c r="N44"/>
+      <c r="O44" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q44"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B45"/>
+      <c r="C45" s="2">
+        <f t="shared" si="4"/>
+        <v>-6</v>
+      </c>
+      <c r="D45" s="2">
+        <f t="shared" si="5"/>
+        <v>-2</v>
+      </c>
+      <c r="E45"/>
+      <c r="F45" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G45" s="1">
+        <v>-20</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J45" s="1">
+        <v>-4</v>
+      </c>
+      <c r="K45" s="1">
+        <v>-4</v>
+      </c>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+      <c r="O45" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q45"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46"/>
+      <c r="C46" s="2">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="D46" s="2">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E46"/>
+      <c r="F46" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G46" s="1">
+        <f t="shared" ref="G46:G51" si="7">J46/4</f>
+        <v>2.5</v>
+      </c>
+      <c r="H46" s="1">
+        <f t="shared" ref="H46:H51" si="8">J46*4</f>
+        <v>40</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J46" s="1">
+        <v>10</v>
+      </c>
+      <c r="K46" s="1">
+        <v>10</v>
+      </c>
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46"/>
+      <c r="O46" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q46"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="2">
+        <f t="shared" si="4"/>
+        <v>2000</v>
+      </c>
+      <c r="D47" s="2">
+        <f t="shared" si="5"/>
+        <v>2000</v>
+      </c>
+      <c r="E47"/>
+      <c r="F47" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G47" s="1">
+        <f t="shared" si="7"/>
+        <v>500</v>
+      </c>
+      <c r="H47" s="1">
+        <f t="shared" si="8"/>
+        <v>8000</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J47" s="1">
+        <v>2000</v>
+      </c>
+      <c r="K47" s="1">
+        <v>1000</v>
+      </c>
+      <c r="L47"/>
+      <c r="M47"/>
+      <c r="N47"/>
+      <c r="O47" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q47"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B48"/>
+      <c r="C48" s="2">
+        <f t="shared" si="4"/>
+        <v>200</v>
+      </c>
+      <c r="D48" s="2">
+        <f t="shared" si="5"/>
+        <v>200</v>
+      </c>
+      <c r="E48"/>
+      <c r="F48" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G48" s="1">
+        <f t="shared" si="7"/>
+        <v>50</v>
+      </c>
+      <c r="H48" s="1">
+        <f t="shared" si="8"/>
+        <v>800</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J48" s="1">
+        <v>200</v>
+      </c>
+      <c r="K48" s="1">
+        <v>100</v>
+      </c>
+      <c r="L48"/>
+      <c r="M48"/>
+      <c r="N48"/>
+      <c r="O48" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q48"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B49"/>
+      <c r="C49" s="2">
+        <f t="shared" si="4"/>
+        <v>200</v>
+      </c>
+      <c r="D49" s="2">
+        <f t="shared" si="5"/>
+        <v>200</v>
+      </c>
+      <c r="E49"/>
+      <c r="F49" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G49" s="1">
+        <f t="shared" si="7"/>
+        <v>50</v>
+      </c>
+      <c r="H49" s="1">
+        <f t="shared" si="8"/>
+        <v>800</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J49" s="1">
+        <v>200</v>
+      </c>
+      <c r="K49" s="1">
+        <v>100</v>
+      </c>
+      <c r="L49"/>
+      <c r="M49"/>
+      <c r="N49"/>
+      <c r="O49" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q49"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B50"/>
+      <c r="C50" s="2">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="D50" s="2">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="E50"/>
+      <c r="F50" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G50" s="1">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="H50" s="1">
+        <f t="shared" si="8"/>
+        <v>80</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J50" s="1">
+        <v>20</v>
+      </c>
+      <c r="K50" s="1">
+        <v>20</v>
+      </c>
+      <c r="L50"/>
+      <c r="M50"/>
+      <c r="N50"/>
+      <c r="O50" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q50"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51"/>
+      <c r="C51" s="2">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="D51" s="2">
+        <f t="shared" si="5"/>
+        <v>1000000</v>
+      </c>
+      <c r="E51"/>
+      <c r="F51" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G51" s="1">
+        <f t="shared" si="7"/>
+        <v>250000</v>
+      </c>
+      <c r="H51" s="1">
+        <f t="shared" si="8"/>
+        <v>4000000</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J51" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K51" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="L51"/>
+      <c r="M51"/>
+      <c r="N51"/>
+      <c r="O51" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P51" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q51"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A52" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B52" s="12"/>
+      <c r="C52" s="13">
+        <f t="shared" si="4"/>
+        <v>0.03</v>
+      </c>
+      <c r="D52" s="13">
+        <f t="shared" si="5"/>
+        <v>0.9</v>
+      </c>
+      <c r="E52" s="12"/>
+      <c r="F52" s="13">
+        <v>3</v>
+      </c>
+      <c r="G52" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="H52" s="11">
+        <v>0.9</v>
+      </c>
+      <c r="I52" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J52" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="K52" s="12"/>
+      <c r="L52" s="12"/>
+      <c r="M52" s="12"/>
+      <c r="N52" s="12"/>
+      <c r="O52" s="11" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P52" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q52"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B53" s="14"/>
+      <c r="C53" s="15">
+        <f t="shared" si="4"/>
+        <v>13000</v>
+      </c>
+      <c r="D53" s="15">
+        <f t="shared" si="5"/>
+        <v>13000</v>
+      </c>
+      <c r="E53" s="14"/>
+      <c r="F53" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="G53" s="14">
+        <f>J53*0.1</f>
+        <v>1300</v>
+      </c>
+      <c r="H53" s="14">
+        <f>J53*10</f>
+        <v>130000</v>
+      </c>
+      <c r="I53" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J53" s="14">
+        <f>J54*5</f>
+        <v>13000</v>
+      </c>
+      <c r="K53" s="14"/>
+      <c r="L53" s="14"/>
+      <c r="M53" s="14"/>
+      <c r="N53" s="14"/>
+      <c r="O53" s="14" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P53" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q53"/>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B54" s="16"/>
+      <c r="C54" s="17">
+        <f t="shared" si="4"/>
+        <v>2600</v>
+      </c>
+      <c r="D54" s="17">
+        <f t="shared" si="5"/>
+        <v>2600</v>
+      </c>
+      <c r="E54" s="16"/>
+      <c r="F54" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="G54" s="5">
+        <f>J54*0.1</f>
+        <v>260</v>
+      </c>
+      <c r="H54" s="5">
+        <f>J54*10</f>
+        <v>26000</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J54" s="5">
+        <v>2600</v>
+      </c>
+      <c r="K54" s="16"/>
+      <c r="L54" s="16"/>
+      <c r="M54" s="16"/>
+      <c r="N54" s="16"/>
+      <c r="O54" s="5" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P54" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q54"/>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B55"/>
+      <c r="C55" s="2">
+        <f t="shared" si="4"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D55" s="2">
+        <f t="shared" si="5"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F55" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0</v>
+      </c>
+      <c r="H55" s="1">
+        <v>1</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J55" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K55"/>
+      <c r="L55"/>
+      <c r="M55"/>
+      <c r="N55"/>
+      <c r="O55" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P55" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q55"/>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56"/>
+      <c r="C56" s="2">
+        <f t="shared" si="4"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D56" s="2">
+        <f t="shared" si="5"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0</v>
+      </c>
+      <c r="H56" s="1">
+        <v>1</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J56" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K56"/>
+      <c r="L56"/>
+      <c r="M56"/>
+      <c r="N56"/>
+      <c r="O56" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P56" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q56"/>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B57"/>
+      <c r="C57" s="2">
+        <f t="shared" si="4"/>
+        <v>0.15</v>
+      </c>
+      <c r="D57" s="2">
+        <f t="shared" si="5"/>
+        <v>0.15</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F57" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G57" s="1">
+        <v>0</v>
+      </c>
+      <c r="H57" s="1">
+        <v>1</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J57" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="K57"/>
+      <c r="L57"/>
+      <c r="M57"/>
+      <c r="N57"/>
+      <c r="O57" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q57"/>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B58"/>
+      <c r="C58" s="2">
+        <f t="shared" si="4"/>
+        <v>0.27999999999999992</v>
+      </c>
+      <c r="D58" s="2">
+        <f t="shared" si="5"/>
+        <v>0.27999999999999992</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F58" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G58" s="1">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1">
+        <v>1</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J58" s="1">
+        <f>1-SUM(J55:J57)</f>
+        <v>0.27999999999999992</v>
+      </c>
+      <c r="K58"/>
+      <c r="L58"/>
+      <c r="M58"/>
+      <c r="N58"/>
+      <c r="O58" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P58" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q58"/>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C59" s="2">
+        <f t="shared" si="4"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D59" s="2">
+        <f t="shared" si="5"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F59" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G59" s="1">
+        <v>0</v>
+      </c>
+      <c r="H59" s="1">
+        <v>1</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J59" s="1">
+        <f>J55</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K59" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L59"/>
+      <c r="M59"/>
+      <c r="N59"/>
+      <c r="O59" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P59" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q59"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B60"/>
+      <c r="C60" s="2">
+        <f t="shared" si="4"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D60" s="2">
+        <f t="shared" si="5"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F60" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G60" s="1">
+        <v>0</v>
+      </c>
+      <c r="H60" s="1">
+        <v>1</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J60" s="1">
+        <f>J56</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K60"/>
+      <c r="L60"/>
+      <c r="M60"/>
+      <c r="N60"/>
+      <c r="O60" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q60"/>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B61"/>
+      <c r="C61" s="2">
+        <f t="shared" si="4"/>
+        <v>0.15</v>
+      </c>
+      <c r="D61" s="2">
+        <f t="shared" si="5"/>
+        <v>0.15</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F61" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0</v>
+      </c>
+      <c r="H61" s="1">
+        <v>1</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J61" s="1">
+        <f>J57</f>
+        <v>0.15</v>
+      </c>
+      <c r="K61"/>
+      <c r="L61"/>
+      <c r="M61"/>
+      <c r="N61"/>
+      <c r="O61" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P61" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q61"/>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B62"/>
+      <c r="C62" s="2">
+        <f t="shared" si="4"/>
+        <v>0.27999999999999992</v>
+      </c>
+      <c r="D62" s="2">
+        <f t="shared" si="5"/>
+        <v>0.27999999999999992</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F62" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G62" s="1">
+        <v>0</v>
+      </c>
+      <c r="H62" s="1">
+        <v>1</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J62" s="1">
+        <f>J58</f>
+        <v>0.27999999999999992</v>
+      </c>
+      <c r="K62"/>
+      <c r="L62"/>
+      <c r="M62"/>
+      <c r="N62"/>
+      <c r="O62" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P62" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q62"/>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C63" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D63" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F63" s="2">
+        <v>3</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0</v>
+      </c>
+      <c r="H63" s="1">
+        <v>1</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J63" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="K63"/>
+      <c r="L63"/>
+      <c r="M63"/>
+      <c r="N63"/>
+      <c r="O63" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P63" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q63"/>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C64" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D64" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F64" s="2">
+        <v>3</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0</v>
+      </c>
+      <c r="H64" s="1">
+        <v>1</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J64" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="K64"/>
+      <c r="L64"/>
+      <c r="M64"/>
+      <c r="N64"/>
+      <c r="O64" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P64" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q64"/>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C65" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D65" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F65" s="2">
+        <v>3</v>
+      </c>
+      <c r="G65" s="1">
+        <v>0</v>
+      </c>
+      <c r="H65" s="1">
+        <v>1</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J65" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="K65"/>
+      <c r="L65"/>
+      <c r="M65"/>
+      <c r="N65"/>
+      <c r="O65" s="1" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P65" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q65"/>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C66" s="8">
+        <f t="shared" si="4"/>
+        <v>0.05</v>
+      </c>
+      <c r="D66" s="8">
+        <f t="shared" si="5"/>
+        <v>0.15</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F66" s="2">
+        <v>5</v>
+      </c>
+      <c r="G66" s="1">
+        <f>MIN(Levers_FullDesign!$D$2:$D$12)</f>
+        <v>0.05</v>
+      </c>
+      <c r="H66" s="1">
+        <f>MAX(Levers_FullDesign!$D$2:$D$14)</f>
+        <v>0.15</v>
+      </c>
+      <c r="I66" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J66" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K66" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="L66"/>
+      <c r="M66"/>
+      <c r="N66"/>
+      <c r="O66" s="1" t="b">
+        <f t="shared" ref="O66:O78" si="9">D66&gt;C66</f>
+        <v>1</v>
+      </c>
+      <c r="P66" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q66" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C67" s="8">
+        <f t="shared" si="4"/>
+        <v>0.05</v>
+      </c>
+      <c r="D67" s="8">
+        <f t="shared" si="5"/>
+        <v>0.15</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F67" s="2">
+        <v>5</v>
+      </c>
+      <c r="G67" s="1">
+        <f>MIN(Levers_FullDesign!$D$2:$D$12)</f>
+        <v>0.05</v>
+      </c>
+      <c r="H67" s="1">
+        <f>MAX(Levers_FullDesign!$D$2:$D$14)</f>
+        <v>0.15</v>
+      </c>
+      <c r="I67" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J67" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K67" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="L67"/>
+      <c r="M67"/>
+      <c r="N67"/>
+      <c r="O67" s="1" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="P67" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C68" s="8">
+        <f t="shared" si="4"/>
+        <v>0.05</v>
+      </c>
+      <c r="D68" s="8">
+        <f t="shared" si="5"/>
+        <v>0.15</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F68" s="2">
+        <v>5</v>
+      </c>
+      <c r="G68" s="1">
+        <f>MIN(Levers_FullDesign!$D$2:$D$12)</f>
+        <v>0.05</v>
+      </c>
+      <c r="H68" s="1">
+        <f>MAX(Levers_FullDesign!$D$2:$D$14)</f>
+        <v>0.15</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J68" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K68" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="L68"/>
+      <c r="M68"/>
+      <c r="N68"/>
+      <c r="O68" s="1" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="P68" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C69" s="2">
+        <f t="shared" si="4"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D69" s="2">
+        <f t="shared" si="5"/>
+        <v>0.43499999999999994</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F69" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G69" s="1">
+        <f>J56</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H69" s="1">
+        <v>1</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J69" s="1">
+        <f>J56</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K69" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L69" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="M69" s="5">
+        <v>1</v>
+      </c>
+      <c r="N69" s="1" t="b">
+        <f t="shared" ref="N69:N78" si="10">C69=D69</f>
+        <v>0</v>
+      </c>
+      <c r="O69" s="1" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="P69" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C70" s="2">
+        <f t="shared" si="4"/>
+        <v>0.15</v>
+      </c>
+      <c r="D70" s="2">
+        <f t="shared" si="5"/>
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F70" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G70" s="1">
+        <f>J57</f>
+        <v>0.15</v>
+      </c>
+      <c r="H70" s="1">
+        <v>1</v>
+      </c>
+      <c r="I70" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J70" s="1">
+        <f>J57</f>
+        <v>0.15</v>
+      </c>
+      <c r="K70" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L70" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="M70" s="5">
+        <v>1</v>
+      </c>
+      <c r="N70" s="1" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="O70" s="1" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="P70" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C71" s="2">
+        <f t="shared" si="4"/>
+        <v>0.27999999999999992</v>
+      </c>
+      <c r="D71" s="2">
+        <f t="shared" si="5"/>
+        <v>0.41999999999999987</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F71" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G71" s="1">
+        <f>J58</f>
+        <v>0.27999999999999992</v>
+      </c>
+      <c r="H71" s="1">
+        <v>1</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J71" s="1">
+        <f>J58</f>
+        <v>0.27999999999999992</v>
+      </c>
+      <c r="K71" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L71" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="M71" s="5">
+        <v>1</v>
+      </c>
+      <c r="N71" s="1" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="O71" s="1" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="P71" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C72" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51</v>
+      </c>
+      <c r="D72" s="2">
+        <f t="shared" si="5"/>
+        <v>2.5</v>
+      </c>
+      <c r="E72"/>
+      <c r="F72" s="2">
+        <v>5</v>
+      </c>
+      <c r="G72" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="H72" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="I72" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J72" s="1">
+        <v>1.49</v>
+      </c>
+      <c r="K72" s="1">
+        <v>1</v>
+      </c>
+      <c r="L72"/>
+      <c r="M72"/>
+      <c r="N72" s="1" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="O72" s="1" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="P72" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C73" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51</v>
+      </c>
+      <c r="D73" s="2">
+        <f t="shared" si="5"/>
+        <v>2.5</v>
+      </c>
+      <c r="E73"/>
+      <c r="F73" s="2">
+        <v>5</v>
+      </c>
+      <c r="G73" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="H73" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J73" s="1">
+        <v>1.49</v>
+      </c>
+      <c r="K73" s="1">
+        <v>1</v>
+      </c>
+      <c r="L73"/>
+      <c r="M73"/>
+      <c r="N73" s="1" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="O73" s="1" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="P73" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C74" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51</v>
+      </c>
+      <c r="D74" s="2">
+        <f t="shared" si="5"/>
+        <v>2.5</v>
+      </c>
+      <c r="E74"/>
+      <c r="F74" s="2">
+        <v>5</v>
+      </c>
+      <c r="G74" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="H74" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="I74" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J74" s="1">
+        <v>1.49</v>
+      </c>
+      <c r="K74" s="1">
+        <v>1</v>
+      </c>
+      <c r="L74"/>
+      <c r="M74"/>
+      <c r="N74" s="1" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="O74" s="1" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="P74" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C75" s="2">
+        <f t="shared" si="4"/>
+        <v>200000</v>
+      </c>
+      <c r="D75" s="2">
+        <f t="shared" si="5"/>
+        <v>200000</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F75" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G75" s="1">
+        <f>J75/10</f>
+        <v>20000</v>
+      </c>
+      <c r="H75" s="1">
+        <f>J75*10</f>
+        <v>2000000</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J75" s="1">
+        <v>200000</v>
+      </c>
+      <c r="K75" s="1">
+        <v>1000</v>
+      </c>
+      <c r="L75"/>
+      <c r="M75"/>
+      <c r="N75" s="1" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="O75" s="1" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P75" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C76" s="2">
+        <f t="shared" si="4"/>
+        <v>200000</v>
+      </c>
+      <c r="D76" s="2">
+        <f t="shared" si="5"/>
+        <v>200000</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F76" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G76" s="1">
+        <f>J76/10</f>
+        <v>20000</v>
+      </c>
+      <c r="H76" s="1">
+        <f>J76*10</f>
+        <v>2000000</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J76" s="1">
+        <v>200000</v>
+      </c>
+      <c r="K76" s="1">
+        <v>1000</v>
+      </c>
+      <c r="L76"/>
+      <c r="M76"/>
+      <c r="N76" s="1" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="O76" s="1" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P76" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C77" s="2">
+        <f t="shared" si="4"/>
+        <v>200000</v>
+      </c>
+      <c r="D77" s="2">
+        <f t="shared" si="5"/>
+        <v>200000</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F77" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G77" s="1">
+        <f>J77/10</f>
+        <v>20000</v>
+      </c>
+      <c r="H77" s="1">
+        <f>J77*10</f>
+        <v>2000000</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J77" s="1">
+        <v>200000</v>
+      </c>
+      <c r="K77" s="1">
+        <v>1000</v>
+      </c>
+      <c r="L77"/>
+      <c r="M77"/>
+      <c r="N77" s="1" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="O77" s="1" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P77" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C78" s="2">
+        <f t="shared" si="4"/>
+        <v>200000</v>
+      </c>
+      <c r="D78" s="2">
+        <f t="shared" si="5"/>
+        <v>200000</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F78" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G78" s="1">
+        <f>J78/10</f>
+        <v>20000</v>
+      </c>
+      <c r="H78" s="1">
+        <f>J78*10</f>
+        <v>2000000</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J78" s="1">
+        <v>200000</v>
+      </c>
+      <c r="K78" s="1">
+        <v>1000</v>
+      </c>
+      <c r="L78"/>
+      <c r="M78"/>
+      <c r="N78" s="1" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="O78" s="1" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P78" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C79" s="2">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D79" s="2">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F79" s="2">
+        <v>0</v>
+      </c>
+      <c r="G79" s="1">
+        <v>1</v>
+      </c>
+      <c r="H79" s="2">
+        <v>3</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J79" s="2">
+        <v>2</v>
+      </c>
+      <c r="K79" s="1">
+        <v>1</v>
+      </c>
+      <c r="P79" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q79" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C80" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D80" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F80" s="2">
+        <v>0</v>
+      </c>
+      <c r="G80" s="1">
+        <v>0</v>
+      </c>
+      <c r="H80" s="1">
+        <v>10000</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J80" s="1">
+        <v>0</v>
+      </c>
+      <c r="K80" s="1">
+        <v>0</v>
+      </c>
+      <c r="P80" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="J81" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J82">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="J83">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J84">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:O78" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMI80"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C62" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5250,6 +9367,46 @@
         <v>219</v>
       </c>
     </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C80" s="2">
+        <f t="shared" ref="C80" si="16">IF(I80="Incerto",MAX(G80,J80-(ABS(F80*J80))),J80)</f>
+        <v>0</v>
+      </c>
+      <c r="D80" s="2">
+        <f t="shared" ref="D80" si="17">IF(I80="Incerto",MIN(H80,J80+(ABS(F80*J80))),J80)</f>
+        <v>0</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F80" s="2">
+        <v>0</v>
+      </c>
+      <c r="G80" s="1">
+        <v>0</v>
+      </c>
+      <c r="H80" s="1">
+        <v>10000</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J80" s="1">
+        <v>0</v>
+      </c>
+      <c r="K80" s="1">
+        <v>0</v>
+      </c>
+      <c r="P80" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:O78" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -5257,12 +9414,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5337,12 +9494,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5426,7 +9583,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -5467,7 +9624,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
@@ -5628,7 +9785,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>

</xml_diff>

<commit_message>
verificação com o Ithink Completa
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
@@ -1275,21 +1275,22 @@
   <dimension ref="A1:AMI84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="A84" sqref="A84"/>
+      <selection pane="bottomRight" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="4" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="2" customWidth="1"/>
     <col min="7" max="9" width="9.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16" width="9.140625" style="1"/>
     <col min="17" max="17" width="36" style="1" customWidth="1"/>
     <col min="18" max="1023" width="9.140625" style="1"/>
@@ -2861,11 +2862,11 @@
       </c>
       <c r="C30" s="2">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>29</v>
@@ -2883,10 +2884,10 @@
         <v>21</v>
       </c>
       <c r="J30" s="1">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="K30" s="1">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="L30"/>
       <c r="M30"/>
@@ -3178,11 +3179,11 @@
       </c>
       <c r="C36" s="2">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="D36" s="2">
         <f t="shared" si="5"/>
-        <v>7.5</v>
+        <v>6</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>29</v>
@@ -3200,10 +3201,10 @@
         <v>38</v>
       </c>
       <c r="J36" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K36" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L36"/>
       <c r="M36"/>
@@ -3895,11 +3896,11 @@
       <c r="B51"/>
       <c r="C51" s="2">
         <f t="shared" si="4"/>
-        <v>1000000</v>
+        <v>1000000000</v>
       </c>
       <c r="D51" s="2">
         <f t="shared" si="5"/>
-        <v>1000000</v>
+        <v>1000000000</v>
       </c>
       <c r="E51"/>
       <c r="F51" s="2">
@@ -3907,17 +3908,18 @@
       </c>
       <c r="G51" s="1">
         <f t="shared" si="7"/>
-        <v>250000</v>
+        <v>250000000</v>
       </c>
       <c r="H51" s="1">
         <f t="shared" si="8"/>
-        <v>4000000</v>
+        <v>4000000000</v>
       </c>
       <c r="I51" s="5" t="s">
         <v>21</v>
       </c>
       <c r="J51" s="1">
-        <v>1000000</v>
+        <f>1000*1000000</f>
+        <v>1000000000</v>
       </c>
       <c r="K51" s="1">
         <v>1000000</v>
@@ -4439,7 +4441,7 @@
       </c>
       <c r="D63" s="2">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>120</v>
@@ -4457,7 +4459,7 @@
         <v>38</v>
       </c>
       <c r="J63" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="K63"/>
       <c r="L63"/>
@@ -4485,7 +4487,7 @@
       </c>
       <c r="D64" s="2">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>120</v>
@@ -4503,7 +4505,7 @@
         <v>38</v>
       </c>
       <c r="J64" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="K64"/>
       <c r="L64"/>
@@ -4531,7 +4533,7 @@
       </c>
       <c r="D65" s="2">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>120</v>
@@ -4549,7 +4551,7 @@
         <v>38</v>
       </c>
       <c r="J65" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="K65"/>
       <c r="L65"/>

</xml_diff>

<commit_message>
quadro de fontes de dados criada, quase completa
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params_testeithink" sheetId="7" r:id="rId1"/>
@@ -1274,11 +1274,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8BAED30-A0E2-440E-98B6-19A75F1BE944}">
   <dimension ref="A1:AMI84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="C42" sqref="C42"/>
+      <selection pane="bottomRight" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5362,11 +5362,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMI80"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C62" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
modificações no arquivo estrategia_v2
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia_v2.xlsx
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="226">
   <si>
     <t>Variavel</t>
   </si>
@@ -774,6 +774,15 @@
   </si>
   <si>
     <t>patentes</t>
+  </si>
+  <si>
+    <t>Forma de Definição</t>
+  </si>
+  <si>
+    <t>FontesUtilizadas</t>
+  </si>
+  <si>
+    <t>(STERMAN 2007)</t>
   </si>
 </sst>
 </file>
@@ -5360,13 +5369,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMI80"/>
+  <dimension ref="A1:AMK80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomRight" activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5380,14 +5389,14 @@
     <col min="10" max="10" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="14" width="6.140625" style="1"/>
     <col min="15" max="15" width="3.5703125" style="1"/>
-    <col min="16" max="16" width="15.140625" style="1"/>
-    <col min="17" max="17" width="36" style="1" customWidth="1"/>
-    <col min="18" max="18" width="8" style="1"/>
-    <col min="19" max="1023" width="6.140625" style="1"/>
-    <col min="1024" max="1025" width="6.140625"/>
+    <col min="16" max="18" width="17.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="36" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8" style="1"/>
+    <col min="21" max="1025" width="6.140625" style="1"/>
+    <col min="1026" max="1027" width="6.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5434,16 +5443,19 @@
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
+        <v>223</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -5492,12 +5504,15 @@
       <c r="P2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="S2" t="s">
         <v>22</v>
       </c>
-      <c r="R2"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T2"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -5546,12 +5561,15 @@
       <c r="P3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="S3" t="s">
         <v>26</v>
       </c>
-      <c r="R3"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T3"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -5600,12 +5618,15 @@
       <c r="P4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="S4" t="s">
         <v>30</v>
       </c>
-      <c r="R4"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T4"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -5654,12 +5675,15 @@
       <c r="P5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="S5" t="s">
         <v>34</v>
       </c>
-      <c r="R5"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T5"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -5715,12 +5739,12 @@
       <c r="P6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="S6" t="s">
         <v>40</v>
       </c>
-      <c r="R6"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T6"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -5769,12 +5793,12 @@
       <c r="P7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="S7" t="s">
         <v>45</v>
       </c>
-      <c r="R7"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T7"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -5823,15 +5847,15 @@
       <c r="P8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="R8" s="1">
         <f>107/0.5</f>
         <v>214</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
@@ -5885,10 +5909,13 @@
         <v>10</v>
       </c>
       <c r="Q9" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="S9" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
@@ -5939,11 +5966,11 @@
       <c r="P10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="S10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -5992,11 +6019,14 @@
       <c r="P11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q11" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="S11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>61</v>
       </c>
@@ -6049,11 +6079,14 @@
       <c r="P12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="Q12" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="S12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>64</v>
       </c>
@@ -6104,9 +6137,9 @@
       <c r="P13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q13"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S13"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>66</v>
       </c>
@@ -6153,9 +6186,12 @@
       <c r="P14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Q14"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q14" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="S14"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
@@ -6208,9 +6244,9 @@
       <c r="P15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q15"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S15"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>70</v>
       </c>
@@ -6259,9 +6295,9 @@
       <c r="P16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q16"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S16"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>72</v>
       </c>
@@ -6314,9 +6350,9 @@
       <c r="P17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q17"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S17"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>74</v>
       </c>
@@ -6365,9 +6401,9 @@
       <c r="P18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q18"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S18"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>76</v>
       </c>
@@ -6416,9 +6452,9 @@
       <c r="P19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q19"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S19"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>78</v>
       </c>
@@ -6467,9 +6503,9 @@
       <c r="P20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q20"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S20"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>80</v>
       </c>
@@ -6522,9 +6558,9 @@
       <c r="P21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q21"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S21"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>82</v>
       </c>
@@ -6573,9 +6609,9 @@
       <c r="P22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q22"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S22"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>84</v>
       </c>
@@ -6626,9 +6662,9 @@
       <c r="P23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q23"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S23"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>87</v>
       </c>
@@ -6683,9 +6719,9 @@
       <c r="P24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q24"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S24"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>89</v>
       </c>
@@ -6734,9 +6770,9 @@
       <c r="P25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q25"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S25"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>91</v>
       </c>
@@ -6789,9 +6825,9 @@
       <c r="P26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q26"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S26"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>93</v>
       </c>
@@ -6842,9 +6878,9 @@
       <c r="P27" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q27"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S27"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>96</v>
       </c>
@@ -6891,9 +6927,9 @@
       <c r="P28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q28"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S28"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>97</v>
       </c>
@@ -6942,9 +6978,9 @@
       <c r="P29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q29"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S29"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>99</v>
       </c>
@@ -6993,9 +7029,9 @@
       <c r="P30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q30"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S30"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>101</v>
       </c>
@@ -7049,9 +7085,9 @@
       <c r="P31" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q31"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S31"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>103</v>
       </c>
@@ -7105,9 +7141,9 @@
       <c r="P32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q32"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S32"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>105</v>
       </c>
@@ -7160,9 +7196,9 @@
       <c r="P33" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q33"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S33"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>107</v>
       </c>
@@ -7211,9 +7247,9 @@
       <c r="P34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q34"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S34"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>109</v>
       </c>
@@ -7259,9 +7295,9 @@
       <c r="P35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q35"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S35"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>111</v>
       </c>
@@ -7307,9 +7343,9 @@
       <c r="P36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q36"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S36"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>113</v>
       </c>
@@ -7357,9 +7393,9 @@
       <c r="P37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q37"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S37"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>116</v>
       </c>
@@ -7407,9 +7443,9 @@
       <c r="P38" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q38"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S38"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>118</v>
       </c>
@@ -7456,9 +7492,9 @@
       <c r="P39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q39"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S39"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>121</v>
       </c>
@@ -7506,9 +7542,9 @@
       <c r="P40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q40"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S40"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>123</v>
       </c>
@@ -7556,9 +7592,9 @@
       <c r="P41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q41"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S41"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>125</v>
       </c>
@@ -7608,9 +7644,9 @@
       <c r="P42" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q42"/>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S42"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>128</v>
       </c>
@@ -7656,9 +7692,9 @@
       <c r="P43" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q43"/>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S43"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>130</v>
       </c>
@@ -7704,9 +7740,9 @@
       <c r="P44" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q44"/>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S44"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>132</v>
       </c>
@@ -7748,9 +7784,9 @@
       <c r="P45" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q45"/>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S45"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>133</v>
       </c>
@@ -7794,9 +7830,9 @@
       <c r="P46" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q46"/>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S46"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>134</v>
       </c>
@@ -7840,9 +7876,9 @@
       <c r="P47" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q47"/>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S47"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>135</v>
       </c>
@@ -7886,9 +7922,9 @@
       <c r="P48" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q48"/>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S48"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>136</v>
       </c>
@@ -7932,9 +7968,9 @@
       <c r="P49" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q49"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S49"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>137</v>
       </c>
@@ -7978,9 +8014,9 @@
       <c r="P50" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q50"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S50"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>138</v>
       </c>
@@ -8024,9 +8060,9 @@
       <c r="P51" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q51"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S51"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>139</v>
       </c>
@@ -8066,9 +8102,11 @@
       <c r="P52" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="Q52"/>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q52" s="11"/>
+      <c r="R52" s="11"/>
+      <c r="S52"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>140</v>
       </c>
@@ -8111,9 +8149,11 @@
       <c r="P53" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="Q53"/>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q53" s="14"/>
+      <c r="R53" s="14"/>
+      <c r="S53"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>141</v>
       </c>
@@ -8155,9 +8195,11 @@
       <c r="P54" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q54"/>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q54" s="5"/>
+      <c r="R54" s="5"/>
+      <c r="S54"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>142</v>
       </c>
@@ -8199,9 +8241,9 @@
       <c r="P55" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q55"/>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S55"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>143</v>
       </c>
@@ -8243,9 +8285,9 @@
       <c r="P56" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q56"/>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S56"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>144</v>
       </c>
@@ -8287,9 +8329,9 @@
       <c r="P57" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q57"/>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S57"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>145</v>
       </c>
@@ -8332,9 +8374,9 @@
       <c r="P58" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q58"/>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S58"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>146</v>
       </c>
@@ -8381,9 +8423,9 @@
       <c r="P59" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q59"/>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S59"/>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>148</v>
       </c>
@@ -8426,9 +8468,9 @@
       <c r="P60" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q60"/>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S60"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>149</v>
       </c>
@@ -8471,9 +8513,9 @@
       <c r="P61" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q61"/>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S61"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>150</v>
       </c>
@@ -8516,9 +8558,9 @@
       <c r="P62" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q62"/>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S62"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>151</v>
       </c>
@@ -8562,9 +8604,9 @@
       <c r="P63" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q63"/>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S63"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>153</v>
       </c>
@@ -8608,9 +8650,9 @@
       <c r="P64" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q64"/>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S64"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>154</v>
       </c>
@@ -8654,9 +8696,9 @@
       <c r="P65" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q65"/>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S65"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>155</v>
       </c>
@@ -8704,11 +8746,11 @@
       <c r="P66" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="Q66" s="1" t="s">
+      <c r="S66" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>159</v>
       </c>
@@ -8757,7 +8799,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>160</v>
       </c>
@@ -8806,7 +8848,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>161</v>
       </c>
@@ -8862,7 +8904,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>163</v>
       </c>
@@ -8918,7 +8960,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>164</v>
       </c>
@@ -8974,7 +9016,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>165</v>
       </c>
@@ -9022,7 +9064,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>167</v>
       </c>
@@ -9070,7 +9112,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>168</v>
       </c>
@@ -9118,7 +9160,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>169</v>
       </c>
@@ -9170,7 +9212,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>171</v>
       </c>
@@ -9222,7 +9264,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>172</v>
       </c>
@@ -9274,7 +9316,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>173</v>
       </c>
@@ -9326,7 +9368,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" ht="135" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>217</v>
       </c>
@@ -9365,11 +9407,11 @@
       <c r="P79" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q79" s="19" t="s">
+      <c r="S79" s="19" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>220</v>
       </c>
@@ -9410,7 +9452,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O78" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>